<commit_message>
updated home page of test data sheet
</commit_message>
<xml_diff>
--- a/GitProject2/src/Test_Data.xlsx
+++ b/GitProject2/src/Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manda\git\eclipseproject\GitProject2\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBB8261-0EAE-407D-A61C-83775ADB237D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14BE146-2C92-4768-AF96-3001259C8152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Element</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t>FMGSITR</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>AGYSITR</t>
   </si>
 </sst>
 </file>
@@ -426,10 +432,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83EAD43F-7383-462E-85C7-99752311FFE7}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,6 +464,14 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added new sheet to test data excel
</commit_message>
<xml_diff>
--- a/GitProject2/src/Test_Data.xlsx
+++ b/GitProject2/src/Test_Data.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manda\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manda\git\eclipseproject\GitProject2\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD9FEB7-2AAE-4A9D-9331-AA65CCA4E35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D298E58-F80E-4D3D-89CE-A28A319236AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Page" sheetId="1" r:id="rId1"/>
     <sheet name="Home_Page" sheetId="2" r:id="rId2"/>
+    <sheet name="Local_Page" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -431,7 +432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83EAD43F-7383-462E-85C7-99752311FFE7}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -472,4 +473,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B13F1CB-F7A8-47CD-ACBA-7CAE7E0F4854}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>